<commit_message>
commint 290924 - add sale data
</commit_message>
<xml_diff>
--- a/result/result.xlsx
+++ b/result/result.xlsx
@@ -342,13 +342,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B207"/>
+  <dimension ref="A1:E207"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A212" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D215" activeCellId="0" sqref="D215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <cols>
+    <col width="43" customWidth="1" style="2" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
@@ -358,7 +361,22 @@
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>Кол-во получено</t>
+          <t>Кол-во получено всего</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Остаток на начало периода</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Продано за период</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Остаток на конец периода</t>
         </is>
       </c>
     </row>
@@ -371,6 +389,15 @@
       <c r="B2" s="3" t="n">
         <v>16</v>
       </c>
+      <c r="C2" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="2">
       <c r="A3" s="3" t="inlineStr">
@@ -381,6 +408,15 @@
       <c r="B3" s="3" t="n">
         <v>28</v>
       </c>
+      <c r="C3" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
@@ -391,6 +427,15 @@
       <c r="B4" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C4" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="2">
       <c r="A5" s="3" t="inlineStr">
@@ -401,6 +446,15 @@
       <c r="B5" s="3" t="n">
         <v>16</v>
       </c>
+      <c r="C5" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="2">
       <c r="A6" s="3" t="inlineStr">
@@ -411,6 +465,15 @@
       <c r="B6" s="3" t="n">
         <v>28</v>
       </c>
+      <c r="C6" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E6" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="2">
       <c r="A7" s="3" t="inlineStr">
@@ -421,6 +484,15 @@
       <c r="B7" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C7" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" ht="12.75" customHeight="1" s="2">
       <c r="A8" s="3" t="inlineStr">
@@ -431,6 +503,15 @@
       <c r="B8" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C8" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" ht="12.75" customHeight="1" s="2">
       <c r="A9" s="3" t="inlineStr">
@@ -441,6 +522,15 @@
       <c r="B9" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C9" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" ht="12.75" customHeight="1" s="2">
       <c r="A10" s="3" t="inlineStr">
@@ -451,6 +541,15 @@
       <c r="B10" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C10" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" s="2">
       <c r="A11" s="3" t="inlineStr">
@@ -461,6 +560,15 @@
       <c r="B11" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C11" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" ht="12.75" customHeight="1" s="2">
       <c r="A12" s="3" t="inlineStr">
@@ -471,6 +579,15 @@
       <c r="B12" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C12" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" ht="12.75" customHeight="1" s="2">
       <c r="A13" s="3" t="inlineStr">
@@ -481,6 +598,15 @@
       <c r="B13" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C13" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" ht="12.75" customHeight="1" s="2">
       <c r="A14" s="3" t="inlineStr">
@@ -491,6 +617,15 @@
       <c r="B14" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C14" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" ht="12.75" customHeight="1" s="2">
       <c r="A15" s="3" t="inlineStr">
@@ -501,6 +636,15 @@
       <c r="B15" s="3" t="n">
         <v>24</v>
       </c>
+      <c r="C15" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="D15" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="E15" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" ht="12.75" customHeight="1" s="2">
       <c r="A16" s="3" t="inlineStr">
@@ -511,6 +655,15 @@
       <c r="B16" s="3" t="n">
         <v>24</v>
       </c>
+      <c r="C16" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E16" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="17" ht="12.75" customHeight="1" s="2">
       <c r="A17" s="3" t="inlineStr">
@@ -521,6 +674,15 @@
       <c r="B17" s="3" t="n">
         <v>64</v>
       </c>
+      <c r="C17" s="3" t="n">
+        <v>60</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="E17" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="18" ht="12.75" customHeight="1" s="2">
       <c r="A18" s="3" t="inlineStr">
@@ -531,6 +693,15 @@
       <c r="B18" s="3" t="n">
         <v>36</v>
       </c>
+      <c r="C18" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="D18" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E18" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="19" ht="12.75" customHeight="1" s="2">
       <c r="A19" s="3" t="inlineStr">
@@ -541,6 +712,15 @@
       <c r="B19" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C19" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E19" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="20" ht="12.75" customHeight="1" s="2">
       <c r="A20" s="3" t="inlineStr">
@@ -551,6 +731,15 @@
       <c r="B20" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C20" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="21" ht="12.75" customHeight="1" s="2">
       <c r="A21" s="3" t="inlineStr">
@@ -561,6 +750,15 @@
       <c r="B21" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C21" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="22" ht="12.75" customHeight="1" s="2">
       <c r="A22" s="3" t="inlineStr">
@@ -571,6 +769,15 @@
       <c r="B22" s="3" t="n">
         <v>16</v>
       </c>
+      <c r="C22" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E22" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="23" ht="12.75" customHeight="1" s="2">
       <c r="A23" s="3" t="inlineStr">
@@ -581,6 +788,15 @@
       <c r="B23" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C23" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="24" ht="12.75" customHeight="1" s="2">
       <c r="A24" s="3" t="inlineStr">
@@ -591,6 +807,15 @@
       <c r="B24" s="3" t="n">
         <v>16</v>
       </c>
+      <c r="C24" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="D24" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E24" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="25" ht="12.75" customHeight="1" s="2">
       <c r="A25" s="3" t="inlineStr">
@@ -601,6 +826,15 @@
       <c r="B25" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C25" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" ht="12.75" customHeight="1" s="2">
       <c r="A26" s="3" t="inlineStr">
@@ -611,6 +845,15 @@
       <c r="B26" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C26" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="27" ht="12.75" customHeight="1" s="2">
       <c r="A27" s="3" t="inlineStr">
@@ -621,6 +864,15 @@
       <c r="B27" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C27" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D27" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" ht="12.75" customHeight="1" s="2">
       <c r="A28" s="3" t="inlineStr">
@@ -631,6 +883,15 @@
       <c r="B28" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C28" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="29" ht="12.75" customHeight="1" s="2">
       <c r="A29" s="3" t="inlineStr">
@@ -641,6 +902,15 @@
       <c r="B29" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C29" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E29" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" ht="12.75" customHeight="1" s="2">
       <c r="A30" s="3" t="inlineStr">
@@ -651,6 +921,15 @@
       <c r="B30" s="3" t="n">
         <v>25</v>
       </c>
+      <c r="C30" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="D30" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E30" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="31" ht="12.75" customHeight="1" s="2">
       <c r="A31" s="3" t="inlineStr">
@@ -661,6 +940,15 @@
       <c r="B31" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C31" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D31" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" ht="12.75" customHeight="1" s="2">
       <c r="A32" s="3" t="inlineStr">
@@ -671,6 +959,15 @@
       <c r="B32" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C32" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D32" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="33" ht="12.75" customHeight="1" s="2">
       <c r="A33" s="3" t="inlineStr">
@@ -681,6 +978,15 @@
       <c r="B33" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C33" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D33" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="34" ht="12.75" customHeight="1" s="2">
       <c r="A34" s="3" t="inlineStr">
@@ -691,6 +997,15 @@
       <c r="B34" s="3" t="n">
         <v>40</v>
       </c>
+      <c r="C34" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="D34" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="E34" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="35" ht="12.75" customHeight="1" s="2">
       <c r="A35" s="3" t="inlineStr">
@@ -701,6 +1016,15 @@
       <c r="B35" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C35" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="36" ht="12.75" customHeight="1" s="2">
       <c r="A36" s="3" t="inlineStr">
@@ -711,6 +1035,15 @@
       <c r="B36" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C36" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="37" ht="12.75" customHeight="1" s="2">
       <c r="A37" s="3" t="inlineStr">
@@ -721,6 +1054,15 @@
       <c r="B37" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C37" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D37" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" ht="12.75" customHeight="1" s="2">
       <c r="A38" s="3" t="inlineStr">
@@ -731,6 +1073,15 @@
       <c r="B38" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C38" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D38" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="39" ht="12.75" customHeight="1" s="2">
       <c r="A39" s="3" t="inlineStr">
@@ -741,6 +1092,15 @@
       <c r="B39" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C39" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="40" ht="12.75" customHeight="1" s="2">
       <c r="A40" s="3" t="inlineStr">
@@ -751,6 +1111,15 @@
       <c r="B40" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C40" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="41" ht="12.75" customHeight="1" s="2">
       <c r="A41" s="3" t="inlineStr">
@@ -761,6 +1130,15 @@
       <c r="B41" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C41" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D41" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="42" ht="12.75" customHeight="1" s="2">
       <c r="A42" s="3" t="inlineStr">
@@ -771,6 +1149,15 @@
       <c r="B42" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C42" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D42" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E42" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="43" ht="12.75" customHeight="1" s="2">
       <c r="A43" s="3" t="inlineStr">
@@ -781,6 +1168,15 @@
       <c r="B43" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C43" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D43" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="44" ht="12.75" customHeight="1" s="2">
       <c r="A44" s="3" t="inlineStr">
@@ -791,6 +1187,15 @@
       <c r="B44" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C44" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D44" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="45" ht="12.75" customHeight="1" s="2">
       <c r="A45" s="3" t="inlineStr">
@@ -801,6 +1206,15 @@
       <c r="B45" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C45" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D45" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="46" ht="12.75" customHeight="1" s="2">
       <c r="A46" s="3" t="inlineStr">
@@ -811,6 +1225,15 @@
       <c r="B46" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C46" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="47" ht="12.75" customHeight="1" s="2">
       <c r="A47" s="3" t="inlineStr">
@@ -821,6 +1244,15 @@
       <c r="B47" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C47" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D47" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="48" ht="12.75" customHeight="1" s="2">
       <c r="A48" s="3" t="inlineStr">
@@ -831,6 +1263,15 @@
       <c r="B48" s="3" t="n">
         <v>10</v>
       </c>
+      <c r="C48" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D48" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E48" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="49" ht="12.75" customHeight="1" s="2">
       <c r="A49" s="3" t="inlineStr">
@@ -841,6 +1282,15 @@
       <c r="B49" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C49" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D49" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E49" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="50" ht="12.75" customHeight="1" s="2">
       <c r="A50" s="3" t="inlineStr">
@@ -851,6 +1301,15 @@
       <c r="B50" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C50" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="51" ht="12.75" customHeight="1" s="2">
       <c r="A51" s="3" t="inlineStr">
@@ -861,6 +1320,15 @@
       <c r="B51" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C51" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="52" ht="12.75" customHeight="1" s="2">
       <c r="A52" s="3" t="inlineStr">
@@ -871,6 +1339,15 @@
       <c r="B52" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C52" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="53" ht="12.75" customHeight="1" s="2">
       <c r="A53" s="3" t="inlineStr">
@@ -881,6 +1358,15 @@
       <c r="B53" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C53" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="54" ht="12.75" customHeight="1" s="2">
       <c r="A54" s="3" t="inlineStr">
@@ -891,6 +1377,15 @@
       <c r="B54" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C54" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" ht="12.75" customHeight="1" s="2">
       <c r="A55" s="3" t="inlineStr">
@@ -901,6 +1396,15 @@
       <c r="B55" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C55" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D55" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="56" ht="12.75" customHeight="1" s="2">
       <c r="A56" s="3" t="inlineStr">
@@ -911,6 +1415,15 @@
       <c r="B56" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C56" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D56" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E56" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="57" ht="12.75" customHeight="1" s="2">
       <c r="A57" s="3" t="inlineStr">
@@ -921,6 +1434,15 @@
       <c r="B57" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C57" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D57" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" ht="12.75" customHeight="1" s="2">
       <c r="A58" s="3" t="inlineStr">
@@ -931,6 +1453,15 @@
       <c r="B58" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C58" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="59" ht="12.75" customHeight="1" s="2">
       <c r="A59" s="3" t="inlineStr">
@@ -941,6 +1472,15 @@
       <c r="B59" s="3" t="n">
         <v>24</v>
       </c>
+      <c r="C59" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="D59" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="E59" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="60" ht="12.75" customHeight="1" s="2">
       <c r="A60" s="3" t="inlineStr">
@@ -951,6 +1491,15 @@
       <c r="B60" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C60" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D60" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E60" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="61" ht="12.75" customHeight="1" s="2">
       <c r="A61" s="3" t="inlineStr">
@@ -961,6 +1510,15 @@
       <c r="B61" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C61" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D61" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" ht="12.75" customHeight="1" s="2">
       <c r="A62" s="3" t="inlineStr">
@@ -971,6 +1529,15 @@
       <c r="B62" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C62" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D62" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="63" ht="12.75" customHeight="1" s="2">
       <c r="A63" s="3" t="inlineStr">
@@ -981,6 +1548,15 @@
       <c r="B63" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C63" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D63" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E63" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="64" ht="12.75" customHeight="1" s="2">
       <c r="A64" s="3" t="inlineStr">
@@ -991,6 +1567,15 @@
       <c r="B64" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C64" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D64" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E64" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="65" ht="12.75" customHeight="1" s="2">
       <c r="A65" s="3" t="inlineStr">
@@ -1001,6 +1586,15 @@
       <c r="B65" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C65" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D65" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E65" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="66" ht="12.75" customHeight="1" s="2">
       <c r="A66" s="3" t="inlineStr">
@@ -1011,6 +1605,15 @@
       <c r="B66" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C66" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D66" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E66" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="67" ht="12.75" customHeight="1" s="2">
       <c r="A67" s="3" t="inlineStr">
@@ -1021,6 +1624,15 @@
       <c r="B67" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C67" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D67" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="68" ht="12.75" customHeight="1" s="2">
       <c r="A68" s="3" t="inlineStr">
@@ -1031,6 +1643,15 @@
       <c r="B68" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C68" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D68" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E68" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="69" ht="12.75" customHeight="1" s="2">
       <c r="A69" s="3" t="inlineStr">
@@ -1041,6 +1662,15 @@
       <c r="B69" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C69" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E69" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="70" ht="12.75" customHeight="1" s="2">
       <c r="A70" s="3" t="inlineStr">
@@ -1051,6 +1681,15 @@
       <c r="B70" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C70" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D70" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="71" ht="12.75" customHeight="1" s="2">
       <c r="A71" s="3" t="inlineStr">
@@ -1061,6 +1700,15 @@
       <c r="B71" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C71" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D71" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E71" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="72" ht="12.75" customHeight="1" s="2">
       <c r="A72" s="3" t="inlineStr">
@@ -1071,6 +1719,15 @@
       <c r="B72" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C72" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D72" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="73" ht="12.75" customHeight="1" s="2">
       <c r="A73" s="3" t="inlineStr">
@@ -1081,6 +1738,15 @@
       <c r="B73" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C73" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D73" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E73" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="74" ht="12.75" customHeight="1" s="2">
       <c r="A74" s="3" t="inlineStr">
@@ -1091,6 +1757,15 @@
       <c r="B74" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C74" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D74" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" ht="12.75" customHeight="1" s="2">
       <c r="A75" s="3" t="inlineStr">
@@ -1101,6 +1776,15 @@
       <c r="B75" s="3" t="n">
         <v>20</v>
       </c>
+      <c r="C75" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="D75" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="E75" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="76" ht="12.75" customHeight="1" s="2">
       <c r="A76" s="3" t="inlineStr">
@@ -1111,6 +1795,15 @@
       <c r="B76" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C76" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D76" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="77" ht="12.75" customHeight="1" s="2">
       <c r="A77" s="3" t="inlineStr">
@@ -1121,6 +1814,15 @@
       <c r="B77" s="3" t="n">
         <v>28</v>
       </c>
+      <c r="C77" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="D77" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="E77" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="78" ht="12.75" customHeight="1" s="2">
       <c r="A78" s="3" t="inlineStr">
@@ -1131,6 +1833,15 @@
       <c r="B78" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C78" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D78" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="79" ht="12.75" customHeight="1" s="2">
       <c r="A79" s="3" t="inlineStr">
@@ -1141,6 +1852,15 @@
       <c r="B79" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C79" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D79" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E79" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="80" ht="12.75" customHeight="1" s="2">
       <c r="A80" s="3" t="inlineStr">
@@ -1151,6 +1871,15 @@
       <c r="B80" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C80" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D80" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E80" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="81" ht="12.75" customHeight="1" s="2">
       <c r="A81" s="3" t="inlineStr">
@@ -1161,6 +1890,15 @@
       <c r="B81" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C81" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D81" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E81" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="82" ht="12.75" customHeight="1" s="2">
       <c r="A82" s="3" t="inlineStr">
@@ -1171,6 +1909,15 @@
       <c r="B82" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C82" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D82" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="83" ht="12.75" customHeight="1" s="2">
       <c r="A83" s="3" t="inlineStr">
@@ -1181,6 +1928,15 @@
       <c r="B83" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="C83" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D83" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="84" ht="12.75" customHeight="1" s="2">
       <c r="A84" s="3" t="inlineStr">
@@ -1191,6 +1947,15 @@
       <c r="B84" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C84" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E84" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="85" ht="12.75" customHeight="1" s="2">
       <c r="A85" s="3" t="inlineStr">
@@ -1201,6 +1966,15 @@
       <c r="B85" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C85" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E85" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="86" ht="12.75" customHeight="1" s="2">
       <c r="A86" s="3" t="inlineStr">
@@ -1211,6 +1985,15 @@
       <c r="B86" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C86" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D86" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E86" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="87" ht="12.75" customHeight="1" s="2">
       <c r="A87" s="3" t="inlineStr">
@@ -1221,6 +2004,15 @@
       <c r="B87" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C87" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D87" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E87" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="88" ht="12.75" customHeight="1" s="2">
       <c r="A88" s="3" t="inlineStr">
@@ -1231,6 +2023,15 @@
       <c r="B88" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C88" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D88" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E88" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="89" ht="12.75" customHeight="1" s="2">
       <c r="A89" s="3" t="inlineStr">
@@ -1241,6 +2042,15 @@
       <c r="B89" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C89" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D89" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90" ht="12.75" customHeight="1" s="2">
       <c r="A90" s="3" t="inlineStr">
@@ -1251,6 +2061,15 @@
       <c r="B90" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C90" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D90" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E90" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="91" ht="12.75" customHeight="1" s="2">
       <c r="A91" s="3" t="inlineStr">
@@ -1261,6 +2080,15 @@
       <c r="B91" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C91" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D91" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E91" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="92" ht="12.75" customHeight="1" s="2">
       <c r="A92" s="3" t="inlineStr">
@@ -1271,6 +2099,15 @@
       <c r="B92" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C92" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D92" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E92" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="93" ht="12.75" customHeight="1" s="2">
       <c r="A93" s="3" t="inlineStr">
@@ -1281,6 +2118,15 @@
       <c r="B93" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C93" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D93" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E93" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="94" ht="12.75" customHeight="1" s="2">
       <c r="A94" s="3" t="inlineStr">
@@ -1291,6 +2137,15 @@
       <c r="B94" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C94" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E94" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="95" ht="12.75" customHeight="1" s="2">
       <c r="A95" s="3" t="inlineStr">
@@ -1301,6 +2156,15 @@
       <c r="B95" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C95" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D95" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E95" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="96" ht="12.75" customHeight="1" s="2">
       <c r="A96" s="3" t="inlineStr">
@@ -1311,6 +2175,15 @@
       <c r="B96" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C96" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D96" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E96" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="97" ht="12.75" customHeight="1" s="2">
       <c r="A97" s="3" t="inlineStr">
@@ -1321,6 +2194,15 @@
       <c r="B97" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C97" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D97" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98" ht="12.75" customHeight="1" s="2">
       <c r="A98" s="3" t="inlineStr">
@@ -1331,6 +2213,15 @@
       <c r="B98" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C98" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D98" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E98" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="99" ht="12.75" customHeight="1" s="2">
       <c r="A99" s="3" t="inlineStr">
@@ -1341,6 +2232,15 @@
       <c r="B99" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C99" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D99" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E99" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="100" ht="12.75" customHeight="1" s="2">
       <c r="A100" s="3" t="inlineStr">
@@ -1351,6 +2251,15 @@
       <c r="B100" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C100" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D100" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="101" ht="12.75" customHeight="1" s="2">
       <c r="A101" s="3" t="inlineStr">
@@ -1361,6 +2270,15 @@
       <c r="B101" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C101" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E101" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="102" ht="12.75" customHeight="1" s="2">
       <c r="A102" s="3" t="inlineStr">
@@ -1371,6 +2289,15 @@
       <c r="B102" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C102" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D102" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E102" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="103" ht="12.75" customHeight="1" s="2">
       <c r="A103" s="3" t="inlineStr">
@@ -1381,6 +2308,15 @@
       <c r="B103" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C103" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D103" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E103" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="104" ht="12.75" customHeight="1" s="2">
       <c r="A104" s="3" t="inlineStr">
@@ -1391,6 +2327,15 @@
       <c r="B104" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C104" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D104" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E104" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="105" ht="12.75" customHeight="1" s="2">
       <c r="A105" s="3" t="inlineStr">
@@ -1401,6 +2346,15 @@
       <c r="B105" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C105" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D105" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E105" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="106" ht="12.75" customHeight="1" s="2">
       <c r="A106" s="3" t="inlineStr">
@@ -1411,6 +2365,15 @@
       <c r="B106" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C106" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E106" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="107" ht="12.75" customHeight="1" s="2">
       <c r="A107" s="3" t="inlineStr">
@@ -1421,6 +2384,15 @@
       <c r="B107" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C107" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E107" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="108" ht="12.75" customHeight="1" s="2">
       <c r="A108" s="3" t="inlineStr">
@@ -1431,6 +2403,15 @@
       <c r="B108" s="3" t="n">
         <v>3</v>
       </c>
+      <c r="C108" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E108" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="109" ht="12.75" customHeight="1" s="2">
       <c r="A109" s="3" t="inlineStr">
@@ -1441,6 +2422,15 @@
       <c r="B109" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C109" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E109" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="110" ht="12.75" customHeight="1" s="2">
       <c r="A110" s="3" t="inlineStr">
@@ -1451,6 +2441,15 @@
       <c r="B110" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C110" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D110" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E110" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="111" ht="12.75" customHeight="1" s="2">
       <c r="A111" s="3" t="inlineStr">
@@ -1461,6 +2460,15 @@
       <c r="B111" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C111" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D111" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E111" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="112" ht="12.75" customHeight="1" s="2">
       <c r="A112" s="3" t="inlineStr">
@@ -1471,6 +2479,15 @@
       <c r="B112" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C112" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D112" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E112" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="113" ht="12.75" customHeight="1" s="2">
       <c r="A113" s="3" t="inlineStr">
@@ -1481,6 +2498,15 @@
       <c r="B113" s="3" t="n">
         <v>11</v>
       </c>
+      <c r="C113" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="D113" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E113" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="114" ht="12.75" customHeight="1" s="2">
       <c r="A114" s="3" t="inlineStr">
@@ -1491,6 +2517,15 @@
       <c r="B114" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C114" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D114" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E114" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="115" ht="12.75" customHeight="1" s="2">
       <c r="A115" s="3" t="inlineStr">
@@ -1501,6 +2536,15 @@
       <c r="B115" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C115" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D115" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E115" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="116" ht="12.75" customHeight="1" s="2">
       <c r="A116" s="3" t="inlineStr">
@@ -1511,6 +2555,15 @@
       <c r="B116" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C116" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D116" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="117" ht="12.75" customHeight="1" s="2">
       <c r="A117" s="3" t="inlineStr">
@@ -1521,6 +2574,15 @@
       <c r="B117" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="C117" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E117" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="118" ht="12.75" customHeight="1" s="2">
       <c r="A118" s="3" t="inlineStr">
@@ -1531,6 +2593,15 @@
       <c r="B118" s="3" t="n">
         <v>6</v>
       </c>
+      <c r="C118" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D118" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E118" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="119" ht="12.75" customHeight="1" s="2">
       <c r="A119" s="3" t="inlineStr">
@@ -1541,6 +2612,15 @@
       <c r="B119" s="3" t="n">
         <v>6</v>
       </c>
+      <c r="C119" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D119" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E119" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="120" ht="12.75" customHeight="1" s="2">
       <c r="A120" s="3" t="inlineStr">
@@ -1551,6 +2631,15 @@
       <c r="B120" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="C120" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D120" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E120" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="121" ht="12.75" customHeight="1" s="2">
       <c r="A121" s="3" t="inlineStr">
@@ -1561,6 +2650,15 @@
       <c r="B121" s="3" t="n">
         <v>6</v>
       </c>
+      <c r="C121" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D121" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E121" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="122" ht="12.75" customHeight="1" s="2">
       <c r="A122" s="3" t="inlineStr">
@@ -1571,6 +2669,15 @@
       <c r="B122" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C122" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E122" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="123" ht="12.75" customHeight="1" s="2">
       <c r="A123" s="3" t="inlineStr">
@@ -1581,6 +2688,15 @@
       <c r="B123" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C123" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D123" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E123" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="124" ht="12.75" customHeight="1" s="2">
       <c r="A124" s="3" t="inlineStr">
@@ -1591,6 +2707,15 @@
       <c r="B124" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C124" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E124" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="125" ht="12.75" customHeight="1" s="2">
       <c r="A125" s="3" t="inlineStr">
@@ -1601,6 +2726,15 @@
       <c r="B125" s="3" t="n">
         <v>6</v>
       </c>
+      <c r="C125" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E125" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="126" ht="12.75" customHeight="1" s="2">
       <c r="A126" s="3" t="inlineStr">
@@ -1611,6 +2745,15 @@
       <c r="B126" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C126" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E126" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="127" ht="12.75" customHeight="1" s="2">
       <c r="A127" s="3" t="inlineStr">
@@ -1621,6 +2764,15 @@
       <c r="B127" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C127" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D127" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E127" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="128" ht="12.75" customHeight="1" s="2">
       <c r="A128" s="3" t="inlineStr">
@@ -1631,6 +2783,15 @@
       <c r="B128" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C128" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D128" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E128" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="129" ht="12.75" customHeight="1" s="2">
       <c r="A129" s="3" t="inlineStr">
@@ -1641,6 +2802,15 @@
       <c r="B129" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C129" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E129" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="130" ht="12.75" customHeight="1" s="2">
       <c r="A130" s="3" t="inlineStr">
@@ -1651,6 +2821,15 @@
       <c r="B130" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C130" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D130" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E130" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="131" ht="12.75" customHeight="1" s="2">
       <c r="A131" s="3" t="inlineStr">
@@ -1661,6 +2840,15 @@
       <c r="B131" s="3" t="n">
         <v>6</v>
       </c>
+      <c r="C131" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E131" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="132" ht="12.75" customHeight="1" s="2">
       <c r="A132" s="3" t="inlineStr">
@@ -1671,6 +2859,15 @@
       <c r="B132" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C132" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E132" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="133" ht="12.75" customHeight="1" s="2">
       <c r="A133" s="3" t="inlineStr">
@@ -1681,6 +2878,15 @@
       <c r="B133" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C133" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E133" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="134" ht="12.75" customHeight="1" s="2">
       <c r="A134" s="3" t="inlineStr">
@@ -1691,6 +2897,15 @@
       <c r="B134" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C134" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E134" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="135" ht="12.75" customHeight="1" s="2">
       <c r="A135" s="3" t="inlineStr">
@@ -1701,6 +2916,15 @@
       <c r="B135" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C135" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D135" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E135" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="136" ht="12.75" customHeight="1" s="2">
       <c r="A136" s="3" t="inlineStr">
@@ -1711,6 +2935,15 @@
       <c r="B136" s="3" t="n">
         <v>16</v>
       </c>
+      <c r="C136" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="D136" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="E136" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="137" ht="12.75" customHeight="1" s="2">
       <c r="A137" s="3" t="inlineStr">
@@ -1721,6 +2954,15 @@
       <c r="B137" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C137" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D137" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E137" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="138" ht="12.75" customHeight="1" s="2">
       <c r="A138" s="3" t="inlineStr">
@@ -1731,6 +2973,15 @@
       <c r="B138" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C138" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E138" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="139" ht="12.75" customHeight="1" s="2">
       <c r="A139" s="3" t="inlineStr">
@@ -1741,6 +2992,15 @@
       <c r="B139" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C139" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D139" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E139" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="140" ht="12.75" customHeight="1" s="2">
       <c r="A140" s="3" t="inlineStr">
@@ -1751,6 +3011,15 @@
       <c r="B140" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="C140" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E140" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="141" ht="12.75" customHeight="1" s="2">
       <c r="A141" s="3" t="inlineStr">
@@ -1761,6 +3030,15 @@
       <c r="B141" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C141" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D141" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E141" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="142" ht="12.75" customHeight="1" s="2">
       <c r="A142" s="3" t="inlineStr">
@@ -1771,6 +3049,15 @@
       <c r="B142" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C142" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E142" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="143" ht="12.75" customHeight="1" s="2">
       <c r="A143" s="3" t="inlineStr">
@@ -1781,6 +3068,15 @@
       <c r="B143" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C143" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D143" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E143" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="144" ht="12.75" customHeight="1" s="2">
       <c r="A144" s="3" t="inlineStr">
@@ -1791,6 +3087,15 @@
       <c r="B144" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C144" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D144" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E144" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="145" ht="12.75" customHeight="1" s="2">
       <c r="A145" s="3" t="inlineStr">
@@ -1801,6 +3106,15 @@
       <c r="B145" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C145" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E145" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="146" ht="12.75" customHeight="1" s="2">
       <c r="A146" s="3" t="inlineStr">
@@ -1811,6 +3125,15 @@
       <c r="B146" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C146" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E146" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="147" ht="12.75" customHeight="1" s="2">
       <c r="A147" s="3" t="inlineStr">
@@ -1821,6 +3144,15 @@
       <c r="B147" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C147" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D147" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E147" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="148" ht="12.75" customHeight="1" s="2">
       <c r="A148" s="3" t="inlineStr">
@@ -1831,6 +3163,15 @@
       <c r="B148" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C148" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E148" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="149" ht="12.75" customHeight="1" s="2">
       <c r="A149" s="3" t="inlineStr">
@@ -1841,6 +3182,15 @@
       <c r="B149" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C149" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D149" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E149" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="150" ht="12.75" customHeight="1" s="2">
       <c r="A150" s="3" t="inlineStr">
@@ -1851,6 +3201,15 @@
       <c r="B150" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C150" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E150" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="151" ht="12.75" customHeight="1" s="2">
       <c r="A151" s="3" t="inlineStr">
@@ -1861,6 +3220,15 @@
       <c r="B151" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C151" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D151" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E151" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="152" ht="12.75" customHeight="1" s="2">
       <c r="A152" s="3" t="inlineStr">
@@ -1871,6 +3239,15 @@
       <c r="B152" s="3" t="n">
         <v>20</v>
       </c>
+      <c r="C152" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="D152" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="E152" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="153" ht="12.75" customHeight="1" s="2">
       <c r="A153" s="3" t="inlineStr">
@@ -1881,6 +3258,15 @@
       <c r="B153" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C153" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D153" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E153" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="154" ht="12.75" customHeight="1" s="2">
       <c r="A154" s="3" t="inlineStr">
@@ -1891,6 +3277,15 @@
       <c r="B154" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C154" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E154" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="155" ht="12.75" customHeight="1" s="2">
       <c r="A155" s="3" t="inlineStr">
@@ -1901,6 +3296,15 @@
       <c r="B155" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C155" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D155" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E155" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="156" ht="12.75" customHeight="1" s="2">
       <c r="A156" s="3" t="inlineStr">
@@ -1911,6 +3315,15 @@
       <c r="B156" s="3" t="n">
         <v>7</v>
       </c>
+      <c r="C156" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D156" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E156" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="157" ht="12.75" customHeight="1" s="2">
       <c r="A157" s="3" t="inlineStr">
@@ -1921,6 +3334,15 @@
       <c r="B157" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C157" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E157" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="158" ht="12.75" customHeight="1" s="2">
       <c r="A158" s="3" t="inlineStr">
@@ -1931,6 +3353,15 @@
       <c r="B158" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C158" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E158" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="159" ht="12.75" customHeight="1" s="2">
       <c r="A159" s="3" t="inlineStr">
@@ -1941,6 +3372,15 @@
       <c r="B159" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C159" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D159" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E159" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="160" ht="12.75" customHeight="1" s="2">
       <c r="A160" s="3" t="inlineStr">
@@ -1951,6 +3391,15 @@
       <c r="B160" s="3" t="n">
         <v>16</v>
       </c>
+      <c r="C160" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="D160" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="E160" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="161" ht="12.75" customHeight="1" s="2">
       <c r="A161" s="3" t="inlineStr">
@@ -1961,6 +3410,15 @@
       <c r="B161" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C161" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D161" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E161" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="162" ht="12.75" customHeight="1" s="2">
       <c r="A162" s="3" t="inlineStr">
@@ -1971,6 +3429,15 @@
       <c r="B162" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C162" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D162" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E162" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="163" ht="12.75" customHeight="1" s="2">
       <c r="A163" s="3" t="inlineStr">
@@ -1981,6 +3448,15 @@
       <c r="B163" s="3" t="n">
         <v>6</v>
       </c>
+      <c r="C163" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E163" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="164" ht="12.75" customHeight="1" s="2">
       <c r="A164" s="3" t="inlineStr">
@@ -1991,6 +3467,15 @@
       <c r="B164" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C164" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D164" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E164" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="165" ht="12.75" customHeight="1" s="2">
       <c r="A165" s="3" t="inlineStr">
@@ -2001,6 +3486,15 @@
       <c r="B165" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C165" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D165" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E165" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="166" ht="12.75" customHeight="1" s="2">
       <c r="A166" s="3" t="inlineStr">
@@ -2011,6 +3505,15 @@
       <c r="B166" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C166" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D166" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E166" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="167" ht="12.75" customHeight="1" s="2">
       <c r="A167" s="3" t="inlineStr">
@@ -2021,6 +3524,15 @@
       <c r="B167" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C167" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D167" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E167" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="168" ht="12.75" customHeight="1" s="2">
       <c r="A168" s="3" t="inlineStr">
@@ -2031,6 +3543,15 @@
       <c r="B168" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C168" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D168" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E168" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="169" ht="12.75" customHeight="1" s="2">
       <c r="A169" s="3" t="inlineStr">
@@ -2041,6 +3562,15 @@
       <c r="B169" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="C169" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D169" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E169" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="170" ht="12.75" customHeight="1" s="2">
       <c r="A170" s="3" t="inlineStr">
@@ -2051,6 +3581,15 @@
       <c r="B170" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C170" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D170" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E170" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="171" ht="12.75" customHeight="1" s="2">
       <c r="A171" s="3" t="inlineStr">
@@ -2061,6 +3600,15 @@
       <c r="B171" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C171" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D171" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E171" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="172" ht="12.75" customHeight="1" s="2">
       <c r="A172" s="3" t="inlineStr">
@@ -2071,6 +3619,15 @@
       <c r="B172" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C172" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D172" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E172" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="173" ht="12.75" customHeight="1" s="2">
       <c r="A173" s="3" t="inlineStr">
@@ -2081,6 +3638,15 @@
       <c r="B173" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C173" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D173" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E173" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="174" ht="12.75" customHeight="1" s="2">
       <c r="A174" s="3" t="inlineStr">
@@ -2091,6 +3657,15 @@
       <c r="B174" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C174" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D174" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E174" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="175" ht="12.75" customHeight="1" s="2">
       <c r="A175" s="3" t="inlineStr">
@@ -2101,6 +3676,15 @@
       <c r="B175" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C175" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D175" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E175" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="176" ht="12.75" customHeight="1" s="2">
       <c r="A176" s="3" t="inlineStr">
@@ -2111,6 +3695,15 @@
       <c r="B176" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C176" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D176" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E176" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="177" ht="12.75" customHeight="1" s="2">
       <c r="A177" s="3" t="inlineStr">
@@ -2121,6 +3714,15 @@
       <c r="B177" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C177" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D177" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E177" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="178" ht="12.75" customHeight="1" s="2">
       <c r="A178" s="3" t="inlineStr">
@@ -2131,6 +3733,15 @@
       <c r="B178" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C178" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D178" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E178" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="179" ht="12.75" customHeight="1" s="2">
       <c r="A179" s="3" t="inlineStr">
@@ -2141,6 +3752,15 @@
       <c r="B179" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C179" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D179" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E179" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="180" ht="12.75" customHeight="1" s="2">
       <c r="A180" s="3" t="inlineStr">
@@ -2151,6 +3771,15 @@
       <c r="B180" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C180" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D180" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E180" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="181" ht="12.75" customHeight="1" s="2">
       <c r="A181" s="3" t="inlineStr">
@@ -2161,6 +3790,15 @@
       <c r="B181" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C181" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D181" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E181" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="182" ht="12.75" customHeight="1" s="2">
       <c r="A182" s="3" t="inlineStr">
@@ -2171,6 +3809,15 @@
       <c r="B182" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C182" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D182" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E182" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="183" ht="12.75" customHeight="1" s="2">
       <c r="A183" s="3" t="inlineStr">
@@ -2181,6 +3828,15 @@
       <c r="B183" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C183" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D183" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E183" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="184" ht="12.75" customHeight="1" s="2">
       <c r="A184" s="3" t="inlineStr">
@@ -2191,6 +3847,15 @@
       <c r="B184" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C184" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D184" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E184" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="185" ht="12.75" customHeight="1" s="2">
       <c r="A185" s="3" t="inlineStr">
@@ -2201,6 +3866,15 @@
       <c r="B185" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C185" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D185" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E185" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="186" ht="12.75" customHeight="1" s="2">
       <c r="A186" s="3" t="inlineStr">
@@ -2211,6 +3885,15 @@
       <c r="B186" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C186" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D186" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E186" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="187" ht="12.75" customHeight="1" s="2">
       <c r="A187" s="3" t="inlineStr">
@@ -2221,6 +3904,15 @@
       <c r="B187" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C187" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D187" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E187" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="188" ht="12.75" customHeight="1" s="2">
       <c r="A188" s="3" t="inlineStr">
@@ -2231,6 +3923,15 @@
       <c r="B188" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C188" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D188" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E188" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="189" ht="12.75" customHeight="1" s="2">
       <c r="A189" s="3" t="inlineStr">
@@ -2241,6 +3942,15 @@
       <c r="B189" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C189" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D189" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E189" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="190" ht="12.75" customHeight="1" s="2">
       <c r="A190" s="3" t="inlineStr">
@@ -2251,6 +3961,15 @@
       <c r="B190" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C190" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D190" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E190" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="191" ht="12.75" customHeight="1" s="2">
       <c r="A191" s="3" t="inlineStr">
@@ -2261,6 +3980,15 @@
       <c r="B191" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C191" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D191" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E191" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="192" ht="12.75" customHeight="1" s="2">
       <c r="A192" s="3" t="inlineStr">
@@ -2271,6 +3999,15 @@
       <c r="B192" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C192" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D192" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E192" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="193" ht="12.75" customHeight="1" s="2">
       <c r="A193" s="3" t="inlineStr">
@@ -2281,6 +4018,15 @@
       <c r="B193" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C193" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D193" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E193" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="194" ht="12.75" customHeight="1" s="2">
       <c r="A194" s="3" t="inlineStr">
@@ -2291,6 +4037,15 @@
       <c r="B194" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C194" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D194" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E194" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="195" ht="12.75" customHeight="1" s="2">
       <c r="A195" s="3" t="inlineStr">
@@ -2301,6 +4056,15 @@
       <c r="B195" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C195" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D195" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E195" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="196" ht="12.75" customHeight="1" s="2">
       <c r="A196" s="3" t="inlineStr">
@@ -2311,6 +4075,15 @@
       <c r="B196" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C196" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D196" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E196" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="197" ht="12.75" customHeight="1" s="2">
       <c r="A197" s="3" t="inlineStr">
@@ -2321,6 +4094,15 @@
       <c r="B197" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C197" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D197" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="E197" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="198" ht="12.75" customHeight="1" s="2">
       <c r="A198" s="3" t="inlineStr">
@@ -2331,6 +4113,15 @@
       <c r="B198" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C198" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D198" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E198" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="199" ht="12.75" customHeight="1" s="2">
       <c r="A199" s="3" t="inlineStr">
@@ -2341,6 +4132,15 @@
       <c r="B199" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C199" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D199" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E199" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="200" ht="12.75" customHeight="1" s="2">
       <c r="A200" s="3" t="inlineStr">
@@ -2351,6 +4151,15 @@
       <c r="B200" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C200" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D200" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E200" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="201" ht="12.75" customHeight="1" s="2">
       <c r="A201" s="3" t="inlineStr">
@@ -2361,6 +4170,15 @@
       <c r="B201" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C201" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D201" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E201" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="202" ht="12.75" customHeight="1" s="2">
       <c r="A202" s="3" t="inlineStr">
@@ -2371,6 +4189,15 @@
       <c r="B202" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C202" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D202" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E202" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="203" ht="12.75" customHeight="1" s="2">
       <c r="A203" s="3" t="inlineStr">
@@ -2381,6 +4208,15 @@
       <c r="B203" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C203" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D203" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E203" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="204" ht="12.75" customHeight="1" s="2">
       <c r="A204" s="3" t="inlineStr">
@@ -2391,6 +4227,15 @@
       <c r="B204" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C204" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D204" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E204" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="205" ht="12.75" customHeight="1" s="2">
       <c r="A205" s="3" t="inlineStr">
@@ -2401,6 +4246,15 @@
       <c r="B205" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C205" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D205" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E205" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="206" ht="12.75" customHeight="1" s="2">
       <c r="A206" s="3" t="inlineStr">
@@ -2409,6 +4263,15 @@
         </is>
       </c>
       <c r="B206" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C206" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D206" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E206" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>